<commit_message>
working-ish for summary tables
</commit_message>
<xml_diff>
--- a/Conception rates by age and country updated.xlsx
+++ b/Conception rates by age and country updated.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/a_baxter_1_research_gla_ac_uk/Documents/R Studio - home folder/teen-preg-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_BAF7BFE20AC7EE95218130F26752ED330E6F9D60" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Under 16" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
   <definedNames>
     <definedName name="Table1Data">[1]table1Data!$A$1:$IV$65536</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -149,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
@@ -467,24 +471,102 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -503,93 +585,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2377,14 +2381,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2:AE2"/>
+      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,7 +2859,7 @@
       <c r="M24" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="L9:M24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L9:M24">
     <sortCondition descending="1" ref="L9:L24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2864,7 +2868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3490,7 +3494,7 @@
       <c r="H30" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="H9:I30">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H9:I30">
     <sortCondition ref="H9:H30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3498,10 +3502,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3986,7 +3990,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="I11:J32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I11:J32">
     <sortCondition descending="1" ref="I11:I32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3995,7 +3999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4389,7 +4393,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BE29"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
@@ -4402,544 +4406,544 @@
       <c r="A1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="50">
+      <c r="B1" s="76">
         <v>2015</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="49">
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="75">
         <v>2014</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="50">
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="76">
         <v>2013</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="49">
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="75">
         <v>2012</v>
       </c>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="50"/>
-      <c r="AD1" s="50"/>
-      <c r="AE1" s="50"/>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="61">
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="76"/>
+      <c r="AF1" s="76"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="72">
         <v>2011</v>
       </c>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="62"/>
-      <c r="AK1" s="62"/>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="63"/>
+      <c r="AI1" s="73"/>
+      <c r="AJ1" s="73"/>
+      <c r="AK1" s="73"/>
+      <c r="AL1" s="73"/>
+      <c r="AM1" s="73"/>
+      <c r="AN1" s="74"/>
       <c r="AO1" s="21"/>
-      <c r="AP1" s="61">
+      <c r="AP1" s="72">
         <v>2010</v>
       </c>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="62"/>
-      <c r="AV1" s="63"/>
+      <c r="AQ1" s="73"/>
+      <c r="AR1" s="73"/>
+      <c r="AS1" s="73"/>
+      <c r="AT1" s="73"/>
+      <c r="AU1" s="73"/>
+      <c r="AV1" s="74"/>
       <c r="AW1" s="21"/>
-      <c r="AX1" s="49">
+      <c r="AX1" s="75">
         <v>2009</v>
       </c>
-      <c r="AY1" s="50"/>
-      <c r="AZ1" s="50"/>
-      <c r="BA1" s="50"/>
-      <c r="BB1" s="50"/>
-      <c r="BC1" s="50"/>
-      <c r="BD1" s="50"/>
-      <c r="BE1" s="51"/>
+      <c r="AY1" s="76"/>
+      <c r="AZ1" s="76"/>
+      <c r="BA1" s="76"/>
+      <c r="BB1" s="76"/>
+      <c r="BC1" s="76"/>
+      <c r="BD1" s="76"/>
+      <c r="BE1" s="77"/>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="43" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="43" t="s">
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="43" t="s">
+      <c r="K2" s="60"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="44" t="s">
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="55"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="43" t="s">
+      <c r="S2" s="60"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="43" t="s">
+      <c r="V2" s="64"/>
+      <c r="W2" s="64"/>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="43" t="s">
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="45"/>
+      <c r="AC2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="43" t="s">
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
+      <c r="AF2" s="64"/>
+      <c r="AG2" s="70"/>
+      <c r="AH2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AI2" s="55"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="43" t="s">
+      <c r="AI2" s="60"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="45"/>
-      <c r="AP2" s="43" t="s">
+      <c r="AL2" s="64"/>
+      <c r="AM2" s="64"/>
+      <c r="AN2" s="64"/>
+      <c r="AO2" s="70"/>
+      <c r="AP2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="55"/>
-      <c r="AR2" s="56"/>
-      <c r="AS2" s="43" t="s">
+      <c r="AQ2" s="60"/>
+      <c r="AR2" s="45"/>
+      <c r="AS2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
-      <c r="AW2" s="45"/>
-      <c r="AX2" s="43" t="s">
+      <c r="AT2" s="64"/>
+      <c r="AU2" s="64"/>
+      <c r="AV2" s="64"/>
+      <c r="AW2" s="70"/>
+      <c r="AX2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="55"/>
-      <c r="AZ2" s="56"/>
-      <c r="BA2" s="43" t="s">
+      <c r="AY2" s="60"/>
+      <c r="AZ2" s="45"/>
+      <c r="BA2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="BB2" s="44"/>
-      <c r="BC2" s="44"/>
-      <c r="BD2" s="44"/>
-      <c r="BE2" s="45"/>
+      <c r="BB2" s="64"/>
+      <c r="BC2" s="64"/>
+      <c r="BD2" s="64"/>
+      <c r="BE2" s="70"/>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="57"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="59"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="47"/>
-      <c r="AE3" s="47"/>
-      <c r="AF3" s="47"/>
-      <c r="AG3" s="48"/>
-      <c r="AH3" s="57"/>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="59"/>
-      <c r="AK3" s="46"/>
-      <c r="AL3" s="47"/>
-      <c r="AM3" s="47"/>
-      <c r="AN3" s="47"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="57"/>
-      <c r="AQ3" s="58"/>
-      <c r="AR3" s="59"/>
-      <c r="AS3" s="46"/>
-      <c r="AT3" s="47"/>
-      <c r="AU3" s="47"/>
-      <c r="AV3" s="47"/>
-      <c r="AW3" s="48"/>
-      <c r="AX3" s="57"/>
-      <c r="AY3" s="58"/>
-      <c r="AZ3" s="59"/>
-      <c r="BA3" s="46"/>
-      <c r="BB3" s="47"/>
-      <c r="BC3" s="47"/>
-      <c r="BD3" s="47"/>
-      <c r="BE3" s="48"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="66"/>
+      <c r="W3" s="66"/>
+      <c r="X3" s="66"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="63"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="66"/>
+      <c r="AE3" s="66"/>
+      <c r="AF3" s="66"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="63"/>
+      <c r="AI3" s="59"/>
+      <c r="AJ3" s="47"/>
+      <c r="AK3" s="68"/>
+      <c r="AL3" s="66"/>
+      <c r="AM3" s="66"/>
+      <c r="AN3" s="66"/>
+      <c r="AO3" s="71"/>
+      <c r="AP3" s="63"/>
+      <c r="AQ3" s="59"/>
+      <c r="AR3" s="47"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="66"/>
+      <c r="AU3" s="66"/>
+      <c r="AV3" s="66"/>
+      <c r="AW3" s="71"/>
+      <c r="AX3" s="63"/>
+      <c r="AY3" s="59"/>
+      <c r="AZ3" s="47"/>
+      <c r="BA3" s="68"/>
+      <c r="BB3" s="66"/>
+      <c r="BC3" s="66"/>
+      <c r="BD3" s="66"/>
+      <c r="BE3" s="71"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="79"/>
+      <c r="B4" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="71"/>
-      <c r="H4" s="55" t="s">
+      <c r="G4" s="69"/>
+      <c r="H4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="77" t="s">
+      <c r="I4" s="54"/>
+      <c r="J4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="80" t="s">
+      <c r="K4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="64" t="s">
+      <c r="M4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="80" t="s">
+      <c r="N4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80" t="s">
+      <c r="O4" s="51"/>
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="64" t="s">
+      <c r="Q4" s="45"/>
+      <c r="R4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="80" t="s">
+      <c r="S4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="74" t="s">
+      <c r="T4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="64" t="s">
+      <c r="U4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="V4" s="80" t="s">
+      <c r="V4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="55"/>
-      <c r="X4" s="80" t="s">
+      <c r="W4" s="60"/>
+      <c r="X4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Y4" s="56"/>
-      <c r="Z4" s="77" t="s">
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AA4" s="80" t="s">
+      <c r="AA4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="74" t="s">
+      <c r="AB4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AC4" s="64" t="s">
+      <c r="AC4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="80" t="s">
+      <c r="AD4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" s="55"/>
-      <c r="AF4" s="80" t="s">
+      <c r="AE4" s="60"/>
+      <c r="AF4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AG4" s="56"/>
-      <c r="AH4" s="64" t="s">
+      <c r="AG4" s="45"/>
+      <c r="AH4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AI4" s="80" t="s">
+      <c r="AI4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="74" t="s">
+      <c r="AJ4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="64" t="s">
+      <c r="AK4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="80" t="s">
+      <c r="AL4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AM4" s="55"/>
-      <c r="AN4" s="80" t="s">
+      <c r="AM4" s="60"/>
+      <c r="AN4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AO4" s="56"/>
-      <c r="AP4" s="64" t="s">
+      <c r="AO4" s="45"/>
+      <c r="AP4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AQ4" s="80" t="s">
+      <c r="AQ4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AR4" s="74" t="s">
+      <c r="AR4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AS4" s="64" t="s">
+      <c r="AS4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AT4" s="80" t="s">
+      <c r="AT4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AU4" s="55"/>
-      <c r="AV4" s="80" t="s">
+      <c r="AU4" s="60"/>
+      <c r="AV4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AW4" s="56"/>
-      <c r="AX4" s="77" t="s">
+      <c r="AW4" s="45"/>
+      <c r="AX4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AY4" s="80" t="s">
+      <c r="AY4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AZ4" s="74" t="s">
+      <c r="AZ4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="BA4" s="81" t="s">
+      <c r="BA4" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="BB4" s="65" t="s">
+      <c r="BB4" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="BC4" s="68"/>
-      <c r="BD4" s="65" t="s">
+      <c r="BC4" s="58"/>
+      <c r="BD4" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="BE4" s="56"/>
+      <c r="BE4" s="45"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="75"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="68"/>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="69"/>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="72"/>
-      <c r="AB5" s="75"/>
-      <c r="AC5" s="65"/>
-      <c r="AD5" s="65"/>
-      <c r="AE5" s="68"/>
-      <c r="AF5" s="65"/>
-      <c r="AG5" s="69"/>
-      <c r="AH5" s="65"/>
-      <c r="AI5" s="72"/>
-      <c r="AJ5" s="75"/>
-      <c r="AK5" s="65"/>
-      <c r="AL5" s="72"/>
-      <c r="AM5" s="68"/>
-      <c r="AN5" s="65"/>
-      <c r="AO5" s="69"/>
-      <c r="AP5" s="65"/>
-      <c r="AQ5" s="72"/>
-      <c r="AR5" s="75"/>
-      <c r="AS5" s="65"/>
-      <c r="AT5" s="72"/>
-      <c r="AU5" s="68"/>
-      <c r="AV5" s="65"/>
-      <c r="AW5" s="69"/>
-      <c r="AX5" s="78"/>
-      <c r="AY5" s="72"/>
-      <c r="AZ5" s="75"/>
-      <c r="BA5" s="65"/>
-      <c r="BB5" s="72"/>
-      <c r="BC5" s="68"/>
-      <c r="BD5" s="65"/>
-      <c r="BE5" s="69"/>
+      <c r="A5" s="79"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="43"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="52"/>
+      <c r="AB5" s="55"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="58"/>
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="46"/>
+      <c r="AH5" s="43"/>
+      <c r="AI5" s="52"/>
+      <c r="AJ5" s="55"/>
+      <c r="AK5" s="43"/>
+      <c r="AL5" s="52"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="43"/>
+      <c r="AO5" s="46"/>
+      <c r="AP5" s="43"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="55"/>
+      <c r="AS5" s="43"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="43"/>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="49"/>
+      <c r="AY5" s="52"/>
+      <c r="AZ5" s="55"/>
+      <c r="BA5" s="43"/>
+      <c r="BB5" s="52"/>
+      <c r="BC5" s="58"/>
+      <c r="BD5" s="43"/>
+      <c r="BE5" s="46"/>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="75"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="65"/>
-      <c r="Y6" s="69"/>
-      <c r="Z6" s="78"/>
-      <c r="AA6" s="72"/>
-      <c r="AB6" s="75"/>
-      <c r="AC6" s="65"/>
-      <c r="AD6" s="65"/>
-      <c r="AE6" s="68"/>
-      <c r="AF6" s="65"/>
-      <c r="AG6" s="69"/>
-      <c r="AH6" s="65"/>
-      <c r="AI6" s="72"/>
-      <c r="AJ6" s="75"/>
-      <c r="AK6" s="65"/>
-      <c r="AL6" s="72"/>
-      <c r="AM6" s="68"/>
-      <c r="AN6" s="65"/>
-      <c r="AO6" s="69"/>
-      <c r="AP6" s="65"/>
-      <c r="AQ6" s="72"/>
-      <c r="AR6" s="75"/>
-      <c r="AS6" s="65"/>
-      <c r="AT6" s="72"/>
-      <c r="AU6" s="68"/>
-      <c r="AV6" s="65"/>
-      <c r="AW6" s="69"/>
-      <c r="AX6" s="78"/>
-      <c r="AY6" s="72"/>
-      <c r="AZ6" s="75"/>
-      <c r="BA6" s="65"/>
-      <c r="BB6" s="72"/>
-      <c r="BC6" s="68"/>
-      <c r="BD6" s="65"/>
-      <c r="BE6" s="69"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="52"/>
+      <c r="T6" s="55"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="43"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="55"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="43"/>
+      <c r="AE6" s="58"/>
+      <c r="AF6" s="43"/>
+      <c r="AG6" s="46"/>
+      <c r="AH6" s="43"/>
+      <c r="AI6" s="52"/>
+      <c r="AJ6" s="55"/>
+      <c r="AK6" s="43"/>
+      <c r="AL6" s="52"/>
+      <c r="AM6" s="58"/>
+      <c r="AN6" s="43"/>
+      <c r="AO6" s="46"/>
+      <c r="AP6" s="43"/>
+      <c r="AQ6" s="52"/>
+      <c r="AR6" s="55"/>
+      <c r="AS6" s="43"/>
+      <c r="AT6" s="52"/>
+      <c r="AU6" s="58"/>
+      <c r="AV6" s="43"/>
+      <c r="AW6" s="46"/>
+      <c r="AX6" s="49"/>
+      <c r="AY6" s="52"/>
+      <c r="AZ6" s="55"/>
+      <c r="BA6" s="43"/>
+      <c r="BB6" s="52"/>
+      <c r="BC6" s="58"/>
+      <c r="BD6" s="43"/>
+      <c r="BE6" s="46"/>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="66"/>
-      <c r="S7" s="73"/>
-      <c r="T7" s="76"/>
-      <c r="U7" s="66"/>
-      <c r="V7" s="66"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="59"/>
-      <c r="Z7" s="79"/>
-      <c r="AA7" s="73"/>
-      <c r="AB7" s="76"/>
-      <c r="AC7" s="66"/>
-      <c r="AD7" s="66"/>
-      <c r="AE7" s="58"/>
-      <c r="AF7" s="66"/>
-      <c r="AG7" s="59"/>
-      <c r="AH7" s="66"/>
-      <c r="AI7" s="73"/>
-      <c r="AJ7" s="76"/>
-      <c r="AK7" s="66"/>
-      <c r="AL7" s="73"/>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="66"/>
-      <c r="AO7" s="59"/>
-      <c r="AP7" s="66"/>
-      <c r="AQ7" s="73"/>
-      <c r="AR7" s="76"/>
-      <c r="AS7" s="66"/>
-      <c r="AT7" s="73"/>
-      <c r="AU7" s="58"/>
-      <c r="AV7" s="66"/>
-      <c r="AW7" s="59"/>
-      <c r="AX7" s="79"/>
-      <c r="AY7" s="73"/>
-      <c r="AZ7" s="76"/>
-      <c r="BA7" s="66"/>
-      <c r="BB7" s="73"/>
-      <c r="BC7" s="58"/>
-      <c r="BD7" s="66"/>
-      <c r="BE7" s="59"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="44"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="50"/>
+      <c r="AA7" s="53"/>
+      <c r="AB7" s="56"/>
+      <c r="AC7" s="44"/>
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="59"/>
+      <c r="AF7" s="44"/>
+      <c r="AG7" s="47"/>
+      <c r="AH7" s="44"/>
+      <c r="AI7" s="53"/>
+      <c r="AJ7" s="56"/>
+      <c r="AK7" s="44"/>
+      <c r="AL7" s="53"/>
+      <c r="AM7" s="59"/>
+      <c r="AN7" s="44"/>
+      <c r="AO7" s="47"/>
+      <c r="AP7" s="44"/>
+      <c r="AQ7" s="53"/>
+      <c r="AR7" s="56"/>
+      <c r="AS7" s="44"/>
+      <c r="AT7" s="53"/>
+      <c r="AU7" s="59"/>
+      <c r="AV7" s="44"/>
+      <c r="AW7" s="47"/>
+      <c r="AX7" s="50"/>
+      <c r="AY7" s="53"/>
+      <c r="AZ7" s="56"/>
+      <c r="BA7" s="44"/>
+      <c r="BB7" s="53"/>
+      <c r="BC7" s="59"/>
+      <c r="BD7" s="44"/>
+      <c r="BE7" s="47"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
@@ -5816,30 +5820,52 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="K23:M29">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K23:M29">
     <sortCondition descending="1" ref="K23"/>
   </sortState>
   <mergeCells count="78">
-    <mergeCell ref="BD4:BD7"/>
-    <mergeCell ref="BE4:BE7"/>
-    <mergeCell ref="AX4:AX7"/>
-    <mergeCell ref="AY4:AY7"/>
-    <mergeCell ref="AZ4:AZ7"/>
-    <mergeCell ref="BA4:BA7"/>
-    <mergeCell ref="BB4:BB7"/>
-    <mergeCell ref="BC4:BC7"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="AL4:AL7"/>
-    <mergeCell ref="AM4:AM7"/>
-    <mergeCell ref="AN4:AN7"/>
-    <mergeCell ref="AO4:AO7"/>
-    <mergeCell ref="AP4:AP7"/>
-    <mergeCell ref="AQ4:AQ7"/>
-    <mergeCell ref="AR4:AR7"/>
-    <mergeCell ref="AS4:AS7"/>
-    <mergeCell ref="AT4:AT7"/>
-    <mergeCell ref="AU4:AU7"/>
-    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="BA2:BE3"/>
+    <mergeCell ref="AX1:BE1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:I3"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="M2:Q3"/>
+    <mergeCell ref="R2:T3"/>
+    <mergeCell ref="U2:Y3"/>
+    <mergeCell ref="Z2:AB3"/>
+    <mergeCell ref="AC2:AG3"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="AH1:AN1"/>
+    <mergeCell ref="AH2:AJ3"/>
+    <mergeCell ref="AK2:AO3"/>
+    <mergeCell ref="AP2:AR3"/>
+    <mergeCell ref="AS2:AW3"/>
+    <mergeCell ref="AP1:AV1"/>
+    <mergeCell ref="AX2:AZ3"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="Y4:Y7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="O4:O7"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="Q4:Q7"/>
+    <mergeCell ref="R4:R7"/>
+    <mergeCell ref="S4:S7"/>
+    <mergeCell ref="T4:T7"/>
     <mergeCell ref="U4:U7"/>
     <mergeCell ref="V4:V7"/>
     <mergeCell ref="W4:W7"/>
@@ -5856,55 +5882,33 @@
     <mergeCell ref="AH4:AH7"/>
     <mergeCell ref="AI4:AI7"/>
     <mergeCell ref="AJ4:AJ7"/>
-    <mergeCell ref="P4:P7"/>
-    <mergeCell ref="Q4:Q7"/>
-    <mergeCell ref="R4:R7"/>
-    <mergeCell ref="S4:S7"/>
-    <mergeCell ref="T4:T7"/>
-    <mergeCell ref="AX2:AZ3"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="Y4:Y7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="O4:O7"/>
-    <mergeCell ref="AH2:AJ3"/>
-    <mergeCell ref="AK2:AO3"/>
-    <mergeCell ref="AP2:AR3"/>
-    <mergeCell ref="AS2:AW3"/>
-    <mergeCell ref="AP1:AV1"/>
-    <mergeCell ref="BA2:BE3"/>
-    <mergeCell ref="AX1:BE1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:I3"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="M2:Q3"/>
-    <mergeCell ref="R2:T3"/>
-    <mergeCell ref="U2:Y3"/>
-    <mergeCell ref="Z2:AB3"/>
-    <mergeCell ref="AC2:AG3"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="Z1:AG1"/>
-    <mergeCell ref="AH1:AN1"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="AL4:AL7"/>
+    <mergeCell ref="AM4:AM7"/>
+    <mergeCell ref="AN4:AN7"/>
+    <mergeCell ref="AO4:AO7"/>
+    <mergeCell ref="AP4:AP7"/>
+    <mergeCell ref="AQ4:AQ7"/>
+    <mergeCell ref="AR4:AR7"/>
+    <mergeCell ref="AS4:AS7"/>
+    <mergeCell ref="AT4:AT7"/>
+    <mergeCell ref="AU4:AU7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="BD4:BD7"/>
+    <mergeCell ref="BE4:BE7"/>
+    <mergeCell ref="AX4:AX7"/>
+    <mergeCell ref="AY4:AY7"/>
+    <mergeCell ref="AZ4:AZ7"/>
+    <mergeCell ref="BA4:BA7"/>
+    <mergeCell ref="BB4:BB7"/>
+    <mergeCell ref="BC4:BC7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6637,18 +6641,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6671,14 +6675,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EB61DB3-56DF-4F4E-BF35-1B81797757F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C935F588-9001-47F7-BF4A-812F4FD3AD14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6693,4 +6689,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EB61DB3-56DF-4F4E-BF35-1B81797757F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>